<commit_message>
Draw LIDAR error charateristic
</commit_message>
<xml_diff>
--- a/0100_Research/0120_Prototypes/TestProtocolTemplate.xlsx
+++ b/0100_Research/0120_Prototypes/TestProtocolTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e675ddd269f32ab/Documents/3e/PGA/git/LoRaSnow/0100_Research/0120_Prototypes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="252" documentId="11_AD4D9D64A577C15A4A5418AA809858665BDEDD8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C1F9166-F7ED-4CC3-93C4-A3177207AB5C}"/>
+  <xr:revisionPtr revIDLastSave="258" documentId="11_AD4D9D64A577C15A4A5418AA809858665BDEDD8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB7A264F-F07F-42A6-B3D3-2356AD6BC8AC}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -176,7 +176,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +204,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -379,7 +386,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -396,12 +403,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -428,6 +429,18 @@
     </xf>
     <xf numFmtId="10" fontId="2" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -961,15 +974,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="13.5" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="24.06640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="86.3984375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="20.59765625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="86.3984375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="20.59765625" style="7" customWidth="1"/>
     <col min="4" max="16384" width="9.06640625" style="3"/>
   </cols>
   <sheetData>
@@ -977,8 +990,8 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -986,61 +999,61 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="16">
+      <c r="B2" s="16"/>
+      <c r="C2" s="14">
         <f>COUNTIF(C3:C986,"Success")/COUNTA(C3:C986)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="11"/>
-    </row>
-    <row r="5" spans="1:3" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.45">
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" spans="1:3" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="11"/>
-    </row>
-    <row r="6" spans="1:3" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.45">
+      <c r="C5" s="9"/>
+    </row>
+    <row r="6" spans="1:3" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="11"/>
-    </row>
-    <row r="7" spans="1:3" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:3" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="11"/>
-    </row>
-    <row r="8" spans="1:3" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.45">
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:3" s="10" customFormat="1" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-    </row>
-    <row r="9" spans="1:3" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.45">
+      <c r="B8" s="17"/>
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" spans="1:3" s="10" customFormat="1" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14" t="s">
+      <c r="B9" s="18"/>
+      <c r="C9" s="12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1049,51 +1062,51 @@
       <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="11"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="9"/>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="11"/>
-    </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+      <c r="C14" s="9"/>
+    </row>
+    <row r="15" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-    </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+      <c r="B15" s="17"/>
+      <c r="C15" s="9"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14" t="s">
+      <c r="B16" s="18"/>
+      <c r="C16" s="12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1102,51 +1115,51 @@
       <c r="A18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="9"/>
     </row>
     <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="11"/>
+      <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.45">
       <c r="A21" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="11"/>
-    </row>
-    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="11"/>
-    </row>
-    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+      <c r="B22" s="17"/>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="14" t="s">
+      <c r="B23" s="18"/>
+      <c r="C23" s="12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1155,51 +1168,51 @@
       <c r="A25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="11"/>
+      <c r="C25" s="9"/>
     </row>
     <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.45">
       <c r="A26" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="11"/>
+      <c r="C26" s="9"/>
     </row>
     <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="11"/>
+      <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.45">
       <c r="A28" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="11"/>
-    </row>
-    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+      <c r="C28" s="9"/>
+    </row>
+    <row r="29" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="11"/>
-    </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+      <c r="B29" s="17"/>
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="14" t="s">
+      <c r="B30" s="18"/>
+      <c r="C30" s="12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1208,51 +1221,51 @@
       <c r="A32" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="11"/>
+      <c r="C32" s="9"/>
     </row>
     <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.45">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="11"/>
+      <c r="C33" s="9"/>
     </row>
     <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.45">
       <c r="A34" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="11"/>
+      <c r="C34" s="9"/>
     </row>
     <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.45">
       <c r="A35" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="11"/>
-    </row>
-    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+      <c r="C35" s="9"/>
+    </row>
+    <row r="36" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A36" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="11"/>
-    </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+      <c r="B36" s="17"/>
+      <c r="C36" s="9"/>
+    </row>
+    <row r="37" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A37" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="14" t="s">
+      <c r="B37" s="18"/>
+      <c r="C37" s="12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1261,51 +1274,51 @@
       <c r="A39" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="11"/>
+      <c r="C39" s="9"/>
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.45">
       <c r="A40" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C40" s="11"/>
+      <c r="C40" s="9"/>
     </row>
     <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.45">
       <c r="A41" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="11"/>
+      <c r="C41" s="9"/>
     </row>
     <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.45">
       <c r="A42" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="11"/>
-    </row>
-    <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+      <c r="C42" s="9"/>
+    </row>
+    <row r="43" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A43" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="11"/>
-    </row>
-    <row r="44" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+      <c r="B43" s="17"/>
+      <c r="C43" s="9"/>
+    </row>
+    <row r="44" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A44" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="13"/>
-      <c r="C44" s="14" t="s">
+      <c r="B44" s="18"/>
+      <c r="C44" s="12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1314,51 +1327,51 @@
       <c r="A46" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C46" s="11"/>
+      <c r="C46" s="9"/>
     </row>
     <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.45">
       <c r="A47" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="11"/>
+      <c r="C47" s="9"/>
     </row>
     <row r="48" spans="1:3" ht="15" x14ac:dyDescent="0.45">
       <c r="A48" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C48" s="11"/>
+      <c r="C48" s="9"/>
     </row>
     <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.45">
       <c r="A49" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C49" s="11"/>
-    </row>
-    <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+      <c r="C49" s="9"/>
+    </row>
+    <row r="50" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A50" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B50" s="10"/>
-      <c r="C50" s="11"/>
-    </row>
-    <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+      <c r="B50" s="17"/>
+      <c r="C50" s="9"/>
+    </row>
+    <row r="51" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A51" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B51" s="13"/>
-      <c r="C51" s="14" t="s">
+      <c r="B51" s="18"/>
+      <c r="C51" s="12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1367,51 +1380,51 @@
       <c r="A53" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C53" s="11"/>
+      <c r="C53" s="9"/>
     </row>
     <row r="54" spans="1:3" ht="15" x14ac:dyDescent="0.45">
       <c r="A54" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B54" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C54" s="11"/>
+      <c r="C54" s="9"/>
     </row>
     <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.45">
       <c r="A55" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B55" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C55" s="11"/>
+      <c r="C55" s="9"/>
     </row>
     <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.45">
       <c r="A56" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B56" s="13" t="s">
+      <c r="B56" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C56" s="11"/>
-    </row>
-    <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+      <c r="C56" s="9"/>
+    </row>
+    <row r="57" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A57" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B57" s="10"/>
-      <c r="C57" s="11"/>
-    </row>
-    <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+      <c r="B57" s="17"/>
+      <c r="C57" s="9"/>
+    </row>
+    <row r="58" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A58" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B58" s="13"/>
-      <c r="C58" s="14" t="s">
+      <c r="B58" s="18"/>
+      <c r="C58" s="12" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>